<commit_message>
Fixed Merged Files and for loop
</commit_message>
<xml_diff>
--- a/absent.xlsx
+++ b/absent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\opiod_list\opioid_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hm/Documents/opioid_list/opioid_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BF4A91-92B5-4786-8475-21C9E9C60E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E537E03E-3A87-BD4E-8163-40CAF70FA2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16200" windowWidth="19185" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -419,7 +419,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03CA00E1-3C54-44A6-A32D-12C2CDB795F5}" name="Table4" displayName="Table4" ref="A1:E35" totalsRowShown="0">
-  <autoFilter ref="A1:E35" xr:uid="{03CA00E1-3C54-44A6-A32D-12C2CDB795F5}"/>
+  <autoFilter ref="A1:E35" xr:uid="{03CA00E1-3C54-44A6-A32D-12C2CDB795F5}">
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="High Dose"/>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C288C53A-B98E-4B1D-98EA-05518B0AE044}" name="drugs_not_found_rxcui"/>
     <tableColumn id="2" xr3:uid="{935BACD2-40AC-41B3-96D7-A73B251258B1}" name="drugs_not_found_name"/>
@@ -755,19 +762,19 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="34.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="4" width="39.54296875" customWidth="1"/>
-    <col min="5" max="5" width="140.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="140.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +791,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -798,7 +805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -812,7 +819,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>10689</v>
       </c>
@@ -826,7 +833,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -840,7 +847,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -854,7 +861,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -871,7 +878,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -888,7 +895,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -902,7 +909,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -916,7 +923,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -930,7 +937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -944,7 +951,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -958,7 +965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -972,7 +979,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -986,7 +993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1003,7 +1010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1017,7 +1024,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1034,7 +1041,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1051,7 +1058,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1099,7 +1106,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1131,7 +1138,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1145,7 +1152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1159,7 +1166,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1174,7 +1181,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1191,7 +1198,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1247,7 +1254,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1261,7 +1268,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>7676</v>
       </c>
@@ -1302,16 +1309,16 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="46.26953125" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -1322,7 +1329,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -1340,7 +1347,7 @@
         <v>4656</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1351,7 +1358,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1362,7 +1369,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1373,7 +1380,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1395,7 +1402,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -1406,7 +1413,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -1428,7 +1435,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -1439,7 +1446,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1472,7 +1479,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1505,7 +1512,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1538,7 +1545,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1560,7 +1567,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>102</v>
       </c>

</xml_diff>